<commit_message>
changed kill to eliminate; changed stick to what is left
</commit_message>
<xml_diff>
--- a/excel/test/shanRoyale2022Data1.xlsx
+++ b/excel/test/shanRoyale2022Data1.xlsx
@@ -2425,7 +2425,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
@@ -2448,14 +2448,64 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>state</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>db</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>chat_id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>elimination_target</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>praveeeenk</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>praveeeenk</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>&lt;dbhelper.DBHelper object at 0x00000156784073A0&gt;</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>258884638</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>